<commit_message>
Cambio de plantilla excel para perfil docente
</commit_message>
<xml_diff>
--- a/public/Uploads/Recursos/temp-perfil-docente.xlsx
+++ b/public/Uploads/Recursos/temp-perfil-docente.xlsx
@@ -9,21 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Laboral" sheetId="1" r:id="rId1"/>
     <sheet name="Academica" sheetId="2" r:id="rId2"/>
     <sheet name="Certificaciones" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja4" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="laboralData" sheetId="5" state="hidden" r:id="rId5"/>
-    <sheet name="academicaData" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="certficacionesData" sheetId="7" state="hidden" r:id="rId7"/>
+    <sheet name="Habilidades" sheetId="8" r:id="rId4"/>
+    <sheet name="Hoja4" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="habilidadesData" sheetId="9" state="hidden" r:id="rId6"/>
+    <sheet name="laboralData" sheetId="5" state="hidden" r:id="rId7"/>
+    <sheet name="academicaData" sheetId="6" state="hidden" r:id="rId8"/>
+    <sheet name="certficacionesData" sheetId="7" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="cargos">Hoja4!$B$1:$C$4</definedName>
+    <definedName name="habilidades">Hoja4!$Q$1:$R$31</definedName>
     <definedName name="idiomas">Hoja4!$F$1:$G$6</definedName>
     <definedName name="materias">Hoja4!$J$1:$K$66</definedName>
+    <definedName name="niveles">Hoja4!$M$1:$N$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="210">
   <si>
     <t>Experiencia Laboral</t>
   </si>
@@ -470,6 +474,200 @@
   </si>
   <si>
     <t>Pera 2</t>
+  </si>
+  <si>
+    <t>Nombre de la Certificación</t>
+  </si>
+  <si>
+    <t>Mandarin</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>Alemán</t>
+  </si>
+  <si>
+    <t>Portugués</t>
+  </si>
+  <si>
+    <t>Año de Certificación</t>
+  </si>
+  <si>
+    <t>Institución en que se certificó</t>
+  </si>
+  <si>
+    <t>Idioma de la Certificación</t>
+  </si>
+  <si>
+    <t>Instrucciones:</t>
+  </si>
+  <si>
+    <t>* La Descripción es Opcional</t>
+  </si>
+  <si>
+    <t>Descripción*</t>
+  </si>
+  <si>
+    <t>Certificaciones</t>
+  </si>
+  <si>
+    <t>lugarTrabajo</t>
+  </si>
+  <si>
+    <t>fechaInicio</t>
+  </si>
+  <si>
+    <t>fechafin</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Anho</t>
+  </si>
+  <si>
+    <t>nombreCert</t>
+  </si>
+  <si>
+    <t>anhoCert</t>
+  </si>
+  <si>
+    <t>institucionCert</t>
+  </si>
+  <si>
+    <t>idiomaCert</t>
+  </si>
+  <si>
+    <t>1 - Para indicar que un registro no tiene fecha fin dejar en blanco
+2- No modifique el orden de las columnas ni hojas del formato
+3 - Solo seleccione valores de las Listas desplegables, de lo contrario esos registros no serán almacenados.</t>
+  </si>
+  <si>
+    <t>Habilidad</t>
+  </si>
+  <si>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>Habilidades</t>
+  </si>
+  <si>
+    <t>Básico</t>
+  </si>
+  <si>
+    <t>Intermedio</t>
+  </si>
+  <si>
+    <t>Avanzado</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server </t>
+  </si>
+  <si>
+    <t>PLSQL</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Java EE</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Chatbot</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>Datawarehouse</t>
+  </si>
+  <si>
+    <t>Power BI</t>
+  </si>
+  <si>
+    <t>Tableu</t>
+  </si>
+  <si>
+    <t>Data Factory</t>
+  </si>
+  <si>
+    <t>ETL</t>
+  </si>
+  <si>
+    <t>Microservicios</t>
+  </si>
+  <si>
+    <t>Domine Driven Design</t>
+  </si>
+  <si>
+    <t>MVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API </t>
+  </si>
+  <si>
+    <t>Scrum</t>
+  </si>
+  <si>
+    <t>Kanbam</t>
+  </si>
+  <si>
+    <t>XP</t>
+  </si>
+  <si>
+    <t>Agile</t>
+  </si>
+  <si>
+    <t>RUP</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>VBA</t>
+  </si>
+  <si>
+    <t>PYTHON</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Haskell</t>
+  </si>
+  <si>
+    <t>idHabilidad</t>
+  </si>
+  <si>
+    <t>idNivel</t>
+  </si>
+  <si>
+    <t>2- No se tomará en cuenta habilidades repetidas.</t>
+  </si>
+  <si>
+    <t>1- Seleccione una habilidad y un nivel de las listas desplegables.</t>
   </si>
   <si>
     <r>
@@ -483,79 +681,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Solo usar se tomarán los registros hasta la fila 50</t>
+      <t>Solo se tomarán en cuenta los registros hasta la fila 50</t>
     </r>
-  </si>
-  <si>
-    <t>Nombre de la Certificación</t>
-  </si>
-  <si>
-    <t>Mandarin</t>
-  </si>
-  <si>
-    <t>Frances</t>
-  </si>
-  <si>
-    <t>Alemán</t>
-  </si>
-  <si>
-    <t>Portugués</t>
-  </si>
-  <si>
-    <t>Año de Certificación</t>
-  </si>
-  <si>
-    <t>Institución en que se certificó</t>
-  </si>
-  <si>
-    <t>Idioma de la Certificación</t>
-  </si>
-  <si>
-    <t>Instrucciones:</t>
-  </si>
-  <si>
-    <t>* La Descripción es Opcional</t>
-  </si>
-  <si>
-    <t>Descripción*</t>
-  </si>
-  <si>
-    <t>Certificaciones</t>
-  </si>
-  <si>
-    <t>lugarTrabajo</t>
-  </si>
-  <si>
-    <t>fechaInicio</t>
-  </si>
-  <si>
-    <t>fechafin</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>Anho</t>
-  </si>
-  <si>
-    <t>nombreCert</t>
-  </si>
-  <si>
-    <t>anhoCert</t>
-  </si>
-  <si>
-    <t>institucionCert</t>
-  </si>
-  <si>
-    <t>idiomaCert</t>
-  </si>
-  <si>
-    <t>1 - Para indicar que un registro no tiene fecha fin dejar en blanco
-2- No modifique el orden de las columnas ni hojas del formato
-3 - Solo seleccione valores de las Listas desplegables, de lo contrario esos registros no serán almacenados.</t>
   </si>
 </sst>
 </file>
@@ -676,7 +803,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -745,11 +872,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -802,6 +979,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -820,15 +1006,29 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,14 +1346,14 @@
   <dimension ref="A1:AG52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="34" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="28" customWidth="1"/>
     <col min="4" max="4" width="50.140625" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" customWidth="1"/>
@@ -1165,36 +1365,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="H3" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1214,20 +1414,20 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
+      <c r="H4" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1235,29 +1435,29 @@
         <v>13</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="2"/>
       <c r="E6" s="5"/>
       <c r="F6" s="4"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="2"/>
       <c r="E7" s="5"/>
       <c r="F7" s="4"/>
@@ -1269,8 +1469,8 @@
     </row>
     <row r="8" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="2"/>
       <c r="E8" s="5"/>
       <c r="F8" s="4"/>
@@ -1282,216 +1482,216 @@
     </row>
     <row r="9" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="2"/>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="2"/>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="2"/>
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="2"/>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="2"/>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="2"/>
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="2"/>
       <c r="E20" s="5"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="2"/>
       <c r="E21" s="5"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="2"/>
       <c r="E22" s="5"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="2"/>
       <c r="E23" s="5"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="2"/>
       <c r="E24" s="5"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="2"/>
       <c r="E25" s="5"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="2"/>
       <c r="E26" s="5"/>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="2"/>
       <c r="E27" s="5"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="2"/>
       <c r="E29" s="5"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="2"/>
       <c r="E30" s="5"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="2"/>
       <c r="E32" s="5"/>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="2"/>
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="2"/>
       <c r="E35" s="5"/>
       <c r="F35" s="11"/>
@@ -1499,8 +1699,8 @@
     </row>
     <row r="36" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="2"/>
       <c r="E36" s="5"/>
       <c r="F36" s="11"/>
@@ -1508,8 +1708,8 @@
     </row>
     <row r="37" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="2"/>
       <c r="E37" s="5"/>
       <c r="F37" s="11"/>
@@ -1517,8 +1717,8 @@
     </row>
     <row r="38" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="2"/>
       <c r="E38" s="5"/>
       <c r="F38" s="11"/>
@@ -1526,8 +1726,8 @@
     </row>
     <row r="39" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="2"/>
       <c r="E39" s="5"/>
       <c r="F39" s="11"/>
@@ -1535,8 +1735,8 @@
     </row>
     <row r="40" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="2"/>
       <c r="E40" s="5"/>
       <c r="F40" s="11"/>
@@ -1544,8 +1744,8 @@
     </row>
     <row r="41" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="2"/>
       <c r="E41" s="5"/>
       <c r="F41" s="11"/>
@@ -1553,8 +1753,8 @@
     </row>
     <row r="42" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
       <c r="F42" s="11"/>
@@ -1562,8 +1762,8 @@
     </row>
     <row r="43" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="2"/>
       <c r="E43" s="5"/>
       <c r="F43" s="11"/>
@@ -1571,8 +1771,8 @@
     </row>
     <row r="44" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="2"/>
       <c r="E44" s="5"/>
       <c r="F44" s="11"/>
@@ -1580,8 +1780,8 @@
     </row>
     <row r="45" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
       <c r="F45" s="11"/>
@@ -1589,8 +1789,8 @@
     </row>
     <row r="46" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
       <c r="F46" s="11"/>
@@ -1598,8 +1798,8 @@
     </row>
     <row r="47" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
       <c r="F47" s="11"/>
@@ -1607,8 +1807,8 @@
     </row>
     <row r="48" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
       <c r="F48" s="11"/>
@@ -1616,8 +1816,8 @@
     </row>
     <row r="49" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="2"/>
       <c r="E49" s="5"/>
       <c r="F49" s="11"/>
@@ -1625,8 +1825,8 @@
     </row>
     <row r="50" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="2"/>
       <c r="E50" s="5"/>
       <c r="F50" s="11"/>
@@ -1674,7 +1874,7 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,26 +1889,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="A1" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1721,10 +1921,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -1748,7 +1948,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="14"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="30"/>
+      <c r="D6" s="24"/>
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -2057,8 +2257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,39 +2271,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="A1" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="A3" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:17" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>153</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -2516,19 +2716,304 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K66"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="41" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="41"/>
+    <col min="4" max="4" width="58.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="37"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="D4" s="43" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="D5" s="44" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="39"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="39"/>
+      <c r="B26" s="39"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="39"/>
+      <c r="B29" s="39"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="39"/>
+      <c r="B48" s="39"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="39"/>
+      <c r="B49" s="39"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="39"/>
+      <c r="B50" s="39"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="39"/>
+      <c r="B51" s="39"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="39"/>
+      <c r="B52" s="39"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="39"/>
+      <c r="B53" s="39"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="39"/>
+      <c r="B54" s="39"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="39"/>
+      <c r="B55" s="39"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="5aVCpSslTu+a+9yrhYvqq027duLBpiMto6ZjkxoxyhFSSPfQW9Ijx6iGUX/NoGSfn1BjuIaPL5CkHzm7AiUyvg==" saltValue="/42LeAXd5VD6fpAi5HpADg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja4!$Q$1:$Q$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>A4:A55</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja4!$M$1:$M$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4:B55</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:S66"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2547,8 +3032,21 @@
       <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="R1" s="22">
+        <v>1</v>
+      </c>
+      <c r="S1" s="35"/>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
@@ -2567,8 +3065,21 @@
       <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>172</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="R2" s="22">
+        <v>2</v>
+      </c>
+      <c r="S2" s="35"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
@@ -2576,7 +3087,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -2587,8 +3098,21 @@
       <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>173</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="R3" s="22">
+        <v>3</v>
+      </c>
+      <c r="S3" s="35"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
@@ -2596,7 +3120,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="3">
         <v>4</v>
@@ -2607,10 +3131,17 @@
       <c r="K4" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q4" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="R4" s="22">
+        <v>4</v>
+      </c>
+      <c r="S4" s="35"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F5" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G5" s="3">
         <v>5</v>
@@ -2621,10 +3152,17 @@
       <c r="K5" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q5" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="R5" s="22">
+        <v>5</v>
+      </c>
+      <c r="S5" s="35"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G6" s="3">
         <v>6</v>
@@ -2635,208 +3173,390 @@
       <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q6" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="R6" s="22">
+        <v>6</v>
+      </c>
+      <c r="S6" s="35"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q7" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="R7" s="22">
+        <v>7</v>
+      </c>
+      <c r="S7" s="35"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J8" s="7" t="s">
         <v>33</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q8" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="R8" s="22">
+        <v>8</v>
+      </c>
+      <c r="S8" s="35"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J9" s="7" t="s">
         <v>35</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q9" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="R9" s="22">
+        <v>9</v>
+      </c>
+      <c r="S9" s="35"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J10" s="7" t="s">
         <v>37</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q10" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="R10" s="22">
+        <v>10</v>
+      </c>
+      <c r="S10" s="35"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J11" s="7" t="s">
         <v>39</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q11" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="R11" s="22">
+        <v>11</v>
+      </c>
+      <c r="S11" s="35"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J12" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q12" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="R12" s="22">
+        <v>12</v>
+      </c>
+      <c r="S12" s="35"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J13" s="7" t="s">
         <v>43</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q13" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="R13" s="22">
+        <v>13</v>
+      </c>
+      <c r="S13" s="35"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J14" s="7" t="s">
         <v>45</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q14" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="R14" s="22">
+        <v>14</v>
+      </c>
+      <c r="S14" s="35"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="Q15" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="R15" s="22">
+        <v>15</v>
+      </c>
+      <c r="S15" s="35"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J16" s="7" t="s">
         <v>49</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q16" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="R16" s="22">
+        <v>16</v>
+      </c>
+      <c r="S16" s="35"/>
+    </row>
+    <row r="17" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J17" s="7" t="s">
         <v>51</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q17" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="R17" s="22">
+        <v>17</v>
+      </c>
+      <c r="S17" s="35"/>
+    </row>
+    <row r="18" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J18" s="7" t="s">
         <v>53</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q18" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="R18" s="22">
+        <v>18</v>
+      </c>
+      <c r="S18" s="35"/>
+    </row>
+    <row r="19" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J19" s="7" t="s">
         <v>55</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q19" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="R19" s="22">
+        <v>19</v>
+      </c>
+      <c r="S19" s="35"/>
+    </row>
+    <row r="20" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J20" s="7" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q20" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="R20" s="22">
+        <v>20</v>
+      </c>
+      <c r="S20" s="35"/>
+    </row>
+    <row r="21" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J21" s="7" t="s">
         <v>59</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q21" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="R21" s="22">
+        <v>21</v>
+      </c>
+      <c r="S21" s="35"/>
+    </row>
+    <row r="22" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J22" s="7" t="s">
         <v>61</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q22" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="R22" s="22">
+        <v>22</v>
+      </c>
+      <c r="S22" s="35"/>
+    </row>
+    <row r="23" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J23" s="7" t="s">
         <v>63</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q23" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="R23" s="22">
+        <v>24</v>
+      </c>
+      <c r="S23" s="35"/>
+    </row>
+    <row r="24" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J24" s="7" t="s">
         <v>65</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q24" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="R24" s="22">
+        <v>25</v>
+      </c>
+      <c r="S24" s="35"/>
+    </row>
+    <row r="25" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J25" s="7" t="s">
         <v>67</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q25" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="R25" s="22">
+        <v>26</v>
+      </c>
+      <c r="S25" s="35"/>
+    </row>
+    <row r="26" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J26" s="7" t="s">
         <v>68</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q26" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="R26" s="22">
+        <v>27</v>
+      </c>
+      <c r="S26" s="35"/>
+    </row>
+    <row r="27" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J27" s="7" t="s">
         <v>70</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q27" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="R27" s="22">
+        <v>28</v>
+      </c>
+      <c r="S27" s="35"/>
+    </row>
+    <row r="28" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J28" s="7" t="s">
         <v>71</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q28" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="R28" s="22">
+        <v>29</v>
+      </c>
+      <c r="S28" s="35"/>
+    </row>
+    <row r="29" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J29" s="7" t="s">
         <v>73</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q29" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="R29" s="22">
+        <v>30</v>
+      </c>
+      <c r="S29" s="35"/>
+    </row>
+    <row r="30" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J30" s="7" t="s">
         <v>75</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="31" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q30" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="R30" s="22">
+        <v>31</v>
+      </c>
+      <c r="S30" s="35"/>
+    </row>
+    <row r="31" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J31" s="7" t="s">
         <v>77</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="Q31" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="R31" s="22">
+        <v>32</v>
+      </c>
+      <c r="S31" s="35"/>
+    </row>
+    <row r="32" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J32" s="7" t="s">
         <v>79</v>
       </c>
@@ -3117,12 +3837,537 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="CQqYpcYc8L97fIbmUWIomA6xGnn/YvPtDVC/S4nfUHtFGZ8eBBu+7vGHNrh7tzQjfaPwYiTMiJL7HAzpe+0Agw==" saltValue="m6n2dnPQb02gBtVaMwecvw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FdluOIeoW4OQGRrFmzyxofUTNxNJNH4sed2Z5KlEEIu8nWiNuCnFqhvcEn3fyyGOa3T6z6jCWJjiBciMLgcZCw==" saltValue="hciGGU+Cz8QGbWyEpsigbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A4,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B2" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B4,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A5,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B5,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A6,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B6,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A7,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B7,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A8,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B8,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A9,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B9,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A10,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B10,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A11,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B11,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A12,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B12,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A13,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B13,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A14,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B14,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A15,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B15,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A16,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B16,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A17,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B17,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A18,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B18,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A19,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B19,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A20,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B20,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A21,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B21,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A22,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B22,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A23,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B23,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A24,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B24,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A25,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B23" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B25,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A26,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B24" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B26,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A27,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B25" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B27,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A28,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B26" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B28,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A29,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B27" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B29,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A30,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B28" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B30,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A31,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B29" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B31,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A32,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B30" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B32,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A33,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B33,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A34,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B32" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B34,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A35,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B35,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A36,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B34" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B36,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A37,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B35" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B37,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A38,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B36" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B38,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A39,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B39,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A40,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B38" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B40,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A41,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B39" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B41,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A42,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B40" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B42,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A43,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B41" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B43,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A44,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B42" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B44,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A45,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B43" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B45,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A46,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B44" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B46,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A47,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B45" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B47,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A48,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B46" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B48,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A49,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B47" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B49,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A50,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B48" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B50,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A51,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B49" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B51,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A52,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B50" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B52,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$A53,habilidades,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="B51" t="str">
+        <f>IFERROR(VLOOKUP(Habilidades!$B53,niveles,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="cR/GuLkQCGumhpStRl4c3FHX+biQPTgyM2JqQ7CYWqRYjKvGL45Zt/sBwRyS1BZ/uKZ9czkcTGrWtgHY011w9g==" saltValue="8RqDy9F92eXMjZbjEuWHMQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
@@ -3141,16 +4386,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="19" t="s">
         <v>160</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>161</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>5</v>
@@ -4175,7 +5420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
@@ -4195,13 +5440,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5092,12 +6337,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5110,16 +6355,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>166</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modificando código de materia en excelazo de perfil docente.
</commit_message>
<xml_diff>
--- a/public/Uploads/Recursos/temp-perfil-docente.xlsx
+++ b/public/Uploads/Recursos/temp-perfil-docente.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eramirez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Laboral" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="materias">Hoja4!$J$1:$K$66</definedName>
     <definedName name="niveles">Hoja4!$M$1:$N$3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="211">
   <si>
     <t>Experiencia Laboral</t>
   </si>
@@ -684,11 +684,14 @@
   <si>
     <t>Año Fin</t>
   </si>
+  <si>
+    <t>HIS115</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1343,28 +1346,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AG52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" style="28" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="50.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="4.5546875" customWidth="1"/>
-    <col min="7" max="7" width="2.5546875" style="4" customWidth="1"/>
-    <col min="8" max="10" width="11.44140625" style="4"/>
-    <col min="11" max="11" width="8.33203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" style="4" customWidth="1"/>
-    <col min="13" max="33" width="11.44140625" style="4"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" customWidth="1"/>
+    <col min="7" max="7" width="2.5703125" style="4" customWidth="1"/>
+    <col min="8" max="10" width="11.42578125" style="4"/>
+    <col min="11" max="11" width="8.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" style="4" customWidth="1"/>
+    <col min="13" max="33" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>207</v>
       </c>
@@ -1372,13 +1376,13 @@
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>0</v>
       </c>
@@ -1396,7 +1400,7 @@
       <c r="K3" s="37"/>
       <c r="L3" s="37"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1422,7 +1426,7 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
     </row>
-    <row r="5" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1441,7 +1445,7 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
@@ -1454,7 +1458,7 @@
       <c r="K6" s="38"/>
       <c r="L6" s="38"/>
     </row>
-    <row r="7" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -1467,7 +1471,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -1480,7 +1484,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
@@ -1488,7 +1492,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -1496,7 +1500,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
@@ -1504,7 +1508,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -1512,7 +1516,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
@@ -1520,7 +1524,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -1528,7 +1532,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
@@ -1536,7 +1540,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -1544,7 +1548,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
@@ -1552,7 +1556,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
@@ -1560,7 +1564,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
@@ -1568,7 +1572,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -1576,7 +1580,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -1584,7 +1588,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
@@ -1592,7 +1596,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -1600,7 +1604,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -1608,7 +1612,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -1616,7 +1620,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
@@ -1624,7 +1628,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -1632,7 +1636,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -1640,7 +1644,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -1648,7 +1652,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
@@ -1656,7 +1660,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -1664,7 +1668,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
@@ -1672,7 +1676,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -1680,7 +1684,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>
@@ -1688,7 +1692,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -1697,7 +1701,7 @@
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="27"/>
       <c r="C36" s="27"/>
@@ -1706,7 +1710,7 @@
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
@@ -1715,7 +1719,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="27"/>
       <c r="C38" s="27"/>
@@ -1724,7 +1728,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
@@ -1733,7 +1737,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="27"/>
       <c r="C40" s="27"/>
@@ -1742,7 +1746,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
@@ -1751,7 +1755,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
     </row>
-    <row r="42" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
@@ -1760,7 +1764,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
     </row>
-    <row r="43" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
@@ -1769,7 +1773,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
@@ -1778,7 +1782,7 @@
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
@@ -1787,7 +1791,7 @@
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
@@ -1796,7 +1800,7 @@
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
@@ -1805,7 +1809,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="27"/>
       <c r="C48" s="27"/>
@@ -1814,7 +1818,7 @@
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="27"/>
       <c r="C49" s="27"/>
@@ -1823,7 +1827,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="27"/>
       <c r="C50" s="27"/>
@@ -1832,11 +1836,11 @@
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
     </row>
@@ -1871,24 +1875,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="41.44140625" customWidth="1"/>
-    <col min="4" max="4" width="90.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="27" style="4" customWidth="1"/>
-    <col min="7" max="23" width="11.44140625" style="4"/>
+    <col min="7" max="23" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>207</v>
       </c>
@@ -1896,13 +1901,13 @@
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>4</v>
       </c>
@@ -1910,7 +1915,7 @@
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1929,7 +1934,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1944,7 +1949,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="14"/>
       <c r="C6" s="2"/>
@@ -1953,7 +1958,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="14"/>
       <c r="C7" s="2"/>
@@ -1961,259 +1966,259 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="14"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="14"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="14"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="14"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="14"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="14"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="14"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="14"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="14"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="14"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="14"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="14"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="14"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="14"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="14"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="14"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="14"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="14"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="14"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="14"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="14"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="14"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="14"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="14"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="14"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="14"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="14"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="14"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="14"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="14"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="14"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="14"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="14"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="14"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="14"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="14"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="14"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="14"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="14"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="14"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="14"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="14"/>
       <c r="C50" s="2"/>
@@ -2255,22 +2260,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="50.5546875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="17" width="11.44140625" style="4"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="17" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>207</v>
       </c>
@@ -2278,13 +2284,13 @@
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>154</v>
       </c>
@@ -2292,7 +2298,7 @@
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
     </row>
-    <row r="4" spans="1:17" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>143</v>
       </c>
@@ -2319,7 +2325,7 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="9"/>
       <c r="C5" s="20"/>
@@ -2327,361 +2333,361 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="9"/>
       <c r="C6" s="20"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="9"/>
       <c r="C7" s="20"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="9"/>
       <c r="C8" s="20"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="9"/>
       <c r="C9" s="20"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="9"/>
       <c r="C10" s="20"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="9"/>
       <c r="C11" s="20"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="9"/>
       <c r="C12" s="20"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="9"/>
       <c r="C13" s="20"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="9"/>
       <c r="C14" s="20"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="9"/>
       <c r="C15" s="20"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="9"/>
       <c r="C16" s="20"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="9"/>
       <c r="C17" s="20"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="9"/>
       <c r="C18" s="20"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="9"/>
       <c r="C19" s="20"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="9"/>
       <c r="C20" s="20"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="9"/>
       <c r="C21" s="20"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="9"/>
       <c r="C22" s="20"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="9"/>
       <c r="C23" s="20"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="9"/>
       <c r="C24" s="20"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="9"/>
       <c r="C25" s="20"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="9"/>
       <c r="C26" s="20"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="9"/>
       <c r="C27" s="20"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="9"/>
       <c r="C28" s="20"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="9"/>
       <c r="C29" s="20"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="9"/>
       <c r="C30" s="20"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="9"/>
       <c r="C31" s="20"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="9"/>
       <c r="C32" s="20"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="9"/>
       <c r="C33" s="20"/>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="9"/>
       <c r="C34" s="20"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="9"/>
       <c r="C35" s="20"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="9"/>
       <c r="C36" s="20"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="9"/>
       <c r="C37" s="20"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="9"/>
       <c r="C38" s="20"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="9"/>
       <c r="C39" s="20"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="9"/>
       <c r="C40" s="20"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="9"/>
       <c r="C41" s="20"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="9"/>
       <c r="C42" s="20"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="9"/>
       <c r="C43" s="20"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="9"/>
       <c r="C44" s="20"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="9"/>
       <c r="C45" s="20"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="9"/>
       <c r="C46" s="20"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="20"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="9"/>
       <c r="C48" s="20"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="9"/>
       <c r="C49" s="20"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="9"/>
       <c r="C50" s="20"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="21"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="21"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="21"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="21"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="21"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="21"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="21"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="21"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="21"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="21"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="21"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="21"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="21"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="21"/>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="21"/>
@@ -2716,22 +2722,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" style="33" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="33"/>
-    <col min="4" max="4" width="58.6640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="33"/>
+    <col min="1" max="1" width="30.140625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="33"/>
+    <col min="4" max="4" width="58.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>207</v>
       </c>
@@ -2740,13 +2747,13 @@
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:5" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>168</v>
       </c>
       <c r="B2" s="44"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>166</v>
       </c>
@@ -2757,217 +2764,217 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="31"/>
       <c r="D4" s="35" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="D5" s="36" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="31"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="31"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="31"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="31"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="31"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="31"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="31"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
       <c r="B13" s="31"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
       <c r="B14" s="31"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="31"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="31"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="31"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
       <c r="B18" s="31"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
       <c r="B19" s="31"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
       <c r="B20" s="31"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="31"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="31"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="31"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="31"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26" s="31"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="31"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
       <c r="B28" s="31"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="31"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="31"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="31"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="31"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="31"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="31"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="31"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="31"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="31"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="31"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="31"/>
       <c r="B40" s="31"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="B41" s="31"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="31"/>
       <c r="B42" s="31"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="31"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="31"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="31"/>
       <c r="B46" s="31"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="31"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="31"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="31"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="31"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="31"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="31"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="31"/>
       <c r="B55" s="31"/>
     </row>
@@ -2979,7 +2986,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Hoja4!$Q$1:$Q$31</xm:f>
@@ -3000,20 +3007,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="B1:S66"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5546875" customWidth="1"/>
-    <col min="10" max="10" width="30.44140625" style="8" customWidth="1"/>
-    <col min="17" max="17" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
@@ -3046,7 +3054,7 @@
       </c>
       <c r="S1" s="29"/>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
@@ -3079,7 +3087,7 @@
       </c>
       <c r="S2" s="29"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -3112,7 +3120,7 @@
       </c>
       <c r="S3" s="29"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
@@ -3139,7 +3147,7 @@
       </c>
       <c r="S4" s="29"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F5" s="3" t="s">
         <v>146</v>
       </c>
@@ -3160,7 +3168,7 @@
       </c>
       <c r="S5" s="29"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F6" s="3" t="s">
         <v>147</v>
       </c>
@@ -3181,7 +3189,7 @@
       </c>
       <c r="S6" s="29"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J7" s="7" t="s">
         <v>29</v>
       </c>
@@ -3196,7 +3204,7 @@
       </c>
       <c r="S7" s="29"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J8" s="7" t="s">
         <v>31</v>
       </c>
@@ -3211,7 +3219,7 @@
       </c>
       <c r="S8" s="29"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J9" s="7" t="s">
         <v>33</v>
       </c>
@@ -3226,7 +3234,7 @@
       </c>
       <c r="S9" s="29"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J10" s="7" t="s">
         <v>35</v>
       </c>
@@ -3241,7 +3249,7 @@
       </c>
       <c r="S10" s="29"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J11" s="7" t="s">
         <v>37</v>
       </c>
@@ -3256,7 +3264,7 @@
       </c>
       <c r="S11" s="29"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J12" s="7" t="s">
         <v>39</v>
       </c>
@@ -3271,7 +3279,7 @@
       </c>
       <c r="S12" s="29"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J13" s="7" t="s">
         <v>41</v>
       </c>
@@ -3286,7 +3294,7 @@
       </c>
       <c r="S13" s="29"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J14" s="7" t="s">
         <v>43</v>
       </c>
@@ -3301,7 +3309,7 @@
       </c>
       <c r="S14" s="29"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J15" s="7" t="s">
         <v>45</v>
       </c>
@@ -3316,7 +3324,7 @@
       </c>
       <c r="S15" s="29"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J16" s="7" t="s">
         <v>47</v>
       </c>
@@ -3331,7 +3339,7 @@
       </c>
       <c r="S16" s="29"/>
     </row>
-    <row r="17" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J17" s="7" t="s">
         <v>49</v>
       </c>
@@ -3346,7 +3354,7 @@
       </c>
       <c r="S17" s="29"/>
     </row>
-    <row r="18" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J18" s="7" t="s">
         <v>51</v>
       </c>
@@ -3361,7 +3369,7 @@
       </c>
       <c r="S18" s="29"/>
     </row>
-    <row r="19" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J19" s="7" t="s">
         <v>53</v>
       </c>
@@ -3376,7 +3384,7 @@
       </c>
       <c r="S19" s="29"/>
     </row>
-    <row r="20" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J20" s="7" t="s">
         <v>55</v>
       </c>
@@ -3391,7 +3399,7 @@
       </c>
       <c r="S20" s="29"/>
     </row>
-    <row r="21" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3406,7 +3414,7 @@
       </c>
       <c r="S21" s="29"/>
     </row>
-    <row r="22" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J22" s="7" t="s">
         <v>59</v>
       </c>
@@ -3421,7 +3429,7 @@
       </c>
       <c r="S22" s="29"/>
     </row>
-    <row r="23" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J23" s="7" t="s">
         <v>61</v>
       </c>
@@ -3436,7 +3444,7 @@
       </c>
       <c r="S23" s="29"/>
     </row>
-    <row r="24" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J24" s="7" t="s">
         <v>63</v>
       </c>
@@ -3451,7 +3459,7 @@
       </c>
       <c r="S24" s="29"/>
     </row>
-    <row r="25" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J25" s="7" t="s">
         <v>65</v>
       </c>
@@ -3466,7 +3474,7 @@
       </c>
       <c r="S25" s="29"/>
     </row>
-    <row r="26" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J26" s="7" t="s">
         <v>66</v>
       </c>
@@ -3481,7 +3489,7 @@
       </c>
       <c r="S26" s="29"/>
     </row>
-    <row r="27" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J27" s="7" t="s">
         <v>68</v>
       </c>
@@ -3496,7 +3504,7 @@
       </c>
       <c r="S27" s="29"/>
     </row>
-    <row r="28" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J28" s="7" t="s">
         <v>69</v>
       </c>
@@ -3511,7 +3519,7 @@
       </c>
       <c r="S28" s="29"/>
     </row>
-    <row r="29" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J29" s="7" t="s">
         <v>71</v>
       </c>
@@ -3526,7 +3534,7 @@
       </c>
       <c r="S29" s="29"/>
     </row>
-    <row r="30" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J30" s="7" t="s">
         <v>73</v>
       </c>
@@ -3541,7 +3549,7 @@
       </c>
       <c r="S30" s="29"/>
     </row>
-    <row r="31" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J31" s="7" t="s">
         <v>75</v>
       </c>
@@ -3556,7 +3564,7 @@
       </c>
       <c r="S31" s="29"/>
     </row>
-    <row r="32" spans="10:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J32" s="7" t="s">
         <v>77</v>
       </c>
@@ -3564,7 +3572,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J33" s="7" t="s">
         <v>79</v>
       </c>
@@ -3572,7 +3580,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J34" s="7" t="s">
         <v>81</v>
       </c>
@@ -3580,7 +3588,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J35" s="7" t="s">
         <v>83</v>
       </c>
@@ -3588,7 +3596,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J36" s="7" t="s">
         <v>84</v>
       </c>
@@ -3596,7 +3604,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J37" s="7" t="s">
         <v>86</v>
       </c>
@@ -3604,15 +3612,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J38" s="7" t="s">
         <v>87</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="10:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J39" s="7" t="s">
         <v>89</v>
       </c>
@@ -3620,7 +3628,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J40" s="7" t="s">
         <v>91</v>
       </c>
@@ -3628,7 +3636,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J41" s="7" t="s">
         <v>93</v>
       </c>
@@ -3636,7 +3644,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J42" s="7" t="s">
         <v>95</v>
       </c>
@@ -3644,7 +3652,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J43" s="7" t="s">
         <v>97</v>
       </c>
@@ -3652,7 +3660,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J44" s="7" t="s">
         <v>99</v>
       </c>
@@ -3660,7 +3668,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J45" s="7" t="s">
         <v>101</v>
       </c>
@@ -3668,7 +3676,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J46" s="7" t="s">
         <v>103</v>
       </c>
@@ -3676,7 +3684,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J47" s="7" t="s">
         <v>105</v>
       </c>
@@ -3684,7 +3692,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J48" s="7" t="s">
         <v>107</v>
       </c>
@@ -3692,7 +3700,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J49" s="7" t="s">
         <v>109</v>
       </c>
@@ -3700,7 +3708,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J50" s="7" t="s">
         <v>111</v>
       </c>
@@ -3708,7 +3716,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J51" s="7" t="s">
         <v>113</v>
       </c>
@@ -3716,7 +3724,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J52" s="7" t="s">
         <v>115</v>
       </c>
@@ -3724,7 +3732,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J53" s="7" t="s">
         <v>117</v>
       </c>
@@ -3732,7 +3740,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J54" s="7" t="s">
         <v>119</v>
       </c>
@@ -3740,7 +3748,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J55" s="7" t="s">
         <v>121</v>
       </c>
@@ -3748,7 +3756,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J56" s="7" t="s">
         <v>123</v>
       </c>
@@ -3756,7 +3764,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J57" s="7" t="s">
         <v>125</v>
       </c>
@@ -3764,7 +3772,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J58" s="7" t="s">
         <v>127</v>
       </c>
@@ -3772,7 +3780,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J59" s="7" t="s">
         <v>129</v>
       </c>
@@ -3780,7 +3788,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J60" s="7" t="s">
         <v>131</v>
       </c>
@@ -3788,7 +3796,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J61" s="7" t="s">
         <v>133</v>
       </c>
@@ -3796,7 +3804,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J62" s="7" t="s">
         <v>135</v>
       </c>
@@ -3804,7 +3812,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="63" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J63" s="7" t="s">
         <v>137</v>
       </c>
@@ -3812,7 +3820,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="64" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J64" s="7" t="s">
         <v>138</v>
       </c>
@@ -3820,7 +3828,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J65" s="7" t="s">
         <v>140</v>
       </c>
@@ -3828,7 +3836,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="10:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J66" s="7" t="s">
         <v>142</v>
       </c>
@@ -3837,22 +3845,23 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FdluOIeoW4OQGRrFmzyxofUTNxNJNH4sed2Z5KlEEIu8nWiNuCnFqhvcEn3fyyGOa3T6z6jCWJjiBciMLgcZCw==" saltValue="hciGGU+Cz8QGbWyEpsigbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="d8i5AVsnPD6u6Z+ZAyThhHkxWQhBxy8SMnXOKeHjcUr58KBqNXt5920D7/J5grhytou+DDra06Yrx0A5/rd8Eg==" saltValue="qbZtmrSbgNvmXVW29TvrsA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>203</v>
       </c>
@@ -3860,7 +3869,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A4,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3870,7 +3879,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A5,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3880,7 +3889,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A6,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3890,7 +3899,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A7,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3900,7 +3909,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A8,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3910,7 +3919,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A9,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3920,7 +3929,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A10,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3930,7 +3939,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A11,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3940,7 +3949,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A12,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3950,7 +3959,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A13,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3960,7 +3969,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A14,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3970,7 +3979,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A15,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3980,7 +3989,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A16,habilidades,2,FALSE),"")</f>
         <v/>
@@ -3990,7 +3999,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A17,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4000,7 +4009,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A18,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4010,7 +4019,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A19,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4020,7 +4029,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A20,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4030,7 +4039,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A21,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4040,7 +4049,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A22,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4050,7 +4059,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A23,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4060,7 +4069,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A24,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4070,7 +4079,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A25,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4080,7 +4089,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A26,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4090,7 +4099,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A27,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4100,7 +4109,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A28,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4110,7 +4119,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A29,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4120,7 +4129,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A30,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4130,7 +4139,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A31,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4140,7 +4149,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A32,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4150,7 +4159,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A33,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4160,7 +4169,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A34,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4170,7 +4179,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A35,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4180,7 +4189,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A36,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4190,7 +4199,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A37,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4200,7 +4209,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A38,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4210,7 +4219,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A39,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4220,7 +4229,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A40,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4230,7 +4239,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A41,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4240,7 +4249,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A42,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4250,7 +4259,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A43,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4260,7 +4269,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A44,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4270,7 +4279,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A45,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4280,7 +4289,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A46,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4290,7 +4299,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A47,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4300,7 +4309,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A48,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4310,7 +4319,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A49,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4320,7 +4329,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A50,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4330,7 +4339,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A51,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4340,7 +4349,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A52,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4350,7 +4359,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IFERROR(VLOOKUP(Habilidades!$A53,habilidades,2,FALSE),"")</f>
         <v/>
@@ -4369,22 +4378,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="22"/>
-    <col min="3" max="3" width="9.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="22"/>
+    <col min="3" max="3" width="9.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>155</v>
       </c>
@@ -4401,7 +4411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="str">
         <f>IF(Laboral!$A5="","",Laboral!$A5)</f>
         <v>Universidad de El Salvador</v>
@@ -4423,7 +4433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="str">
         <f>IF(Laboral!$A6="","",Laboral!$A6)</f>
         <v/>
@@ -4445,7 +4455,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="str">
         <f>IF(Laboral!$A7="","",Laboral!$A7)</f>
         <v/>
@@ -4467,7 +4477,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="str">
         <f>IF(Laboral!$A8="","",Laboral!$A8)</f>
         <v/>
@@ -4489,7 +4499,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="str">
         <f>IF(Laboral!$A9="","",Laboral!$A9)</f>
         <v/>
@@ -4511,7 +4521,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="str">
         <f>IF(Laboral!$A10="","",Laboral!$A10)</f>
         <v/>
@@ -4533,7 +4543,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="str">
         <f>IF(Laboral!$A11="","",Laboral!$A11)</f>
         <v/>
@@ -4555,7 +4565,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="str">
         <f>IF(Laboral!$A12="","",Laboral!$A12)</f>
         <v/>
@@ -4577,7 +4587,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="str">
         <f>IF(Laboral!$A13="","",Laboral!$A13)</f>
         <v/>
@@ -4599,7 +4609,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="str">
         <f>IF(Laboral!$A14="","",Laboral!$A14)</f>
         <v/>
@@ -4621,7 +4631,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="str">
         <f>IF(Laboral!$A15="","",Laboral!$A15)</f>
         <v/>
@@ -4643,7 +4653,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="str">
         <f>IF(Laboral!$A16="","",Laboral!$A16)</f>
         <v/>
@@ -4665,7 +4675,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="str">
         <f>IF(Laboral!$A17="","",Laboral!$A17)</f>
         <v/>
@@ -4687,7 +4697,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="str">
         <f>IF(Laboral!$A18="","",Laboral!$A18)</f>
         <v/>
@@ -4709,7 +4719,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="str">
         <f>IF(Laboral!$A19="","",Laboral!$A19)</f>
         <v/>
@@ -4731,7 +4741,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="str">
         <f>IF(Laboral!$A20="","",Laboral!$A20)</f>
         <v/>
@@ -4753,7 +4763,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="str">
         <f>IF(Laboral!$A21="","",Laboral!$A21)</f>
         <v/>
@@ -4775,7 +4785,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="str">
         <f>IF(Laboral!$A22="","",Laboral!$A22)</f>
         <v/>
@@ -4797,7 +4807,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="str">
         <f>IF(Laboral!$A23="","",Laboral!$A23)</f>
         <v/>
@@ -4819,7 +4829,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="str">
         <f>IF(Laboral!$A24="","",Laboral!$A24)</f>
         <v/>
@@ -4841,7 +4851,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="str">
         <f>IF(Laboral!$A25="","",Laboral!$A25)</f>
         <v/>
@@ -4863,7 +4873,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="str">
         <f>IF(Laboral!$A26="","",Laboral!$A26)</f>
         <v/>
@@ -4885,7 +4895,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="str">
         <f>IF(Laboral!$A27="","",Laboral!$A27)</f>
         <v/>
@@ -4907,7 +4917,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="str">
         <f>IF(Laboral!$A28="","",Laboral!$A28)</f>
         <v/>
@@ -4929,7 +4939,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="str">
         <f>IF(Laboral!$A29="","",Laboral!$A29)</f>
         <v/>
@@ -4951,7 +4961,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="str">
         <f>IF(Laboral!$A30="","",Laboral!$A30)</f>
         <v/>
@@ -4973,7 +4983,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="str">
         <f>IF(Laboral!$A31="","",Laboral!$A31)</f>
         <v/>
@@ -4995,7 +5005,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="str">
         <f>IF(Laboral!$A32="","",Laboral!$A32)</f>
         <v/>
@@ -5017,7 +5027,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="str">
         <f>IF(Laboral!$A33="","",Laboral!$A33)</f>
         <v/>
@@ -5039,7 +5049,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="str">
         <f>IF(Laboral!$A34="","",Laboral!$A34)</f>
         <v/>
@@ -5061,7 +5071,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="str">
         <f>IF(Laboral!$A35="","",Laboral!$A35)</f>
         <v/>
@@ -5083,7 +5093,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="str">
         <f>IF(Laboral!$A36="","",Laboral!$A36)</f>
         <v/>
@@ -5105,7 +5115,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="str">
         <f>IF(Laboral!$A37="","",Laboral!$A37)</f>
         <v/>
@@ -5127,7 +5137,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="str">
         <f>IF(Laboral!$A38="","",Laboral!$A38)</f>
         <v/>
@@ -5149,7 +5159,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="str">
         <f>IF(Laboral!$A39="","",Laboral!$A39)</f>
         <v/>
@@ -5171,7 +5181,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="str">
         <f>IF(Laboral!$A40="","",Laboral!$A40)</f>
         <v/>
@@ -5193,7 +5203,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="str">
         <f>IF(Laboral!$A41="","",Laboral!$A41)</f>
         <v/>
@@ -5215,7 +5225,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="str">
         <f>IF(Laboral!$A42="","",Laboral!$A42)</f>
         <v/>
@@ -5237,7 +5247,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="str">
         <f>IF(Laboral!$A43="","",Laboral!$A43)</f>
         <v/>
@@ -5259,7 +5269,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="str">
         <f>IF(Laboral!$A44="","",Laboral!$A44)</f>
         <v/>
@@ -5281,7 +5291,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="str">
         <f>IF(Laboral!$A45="","",Laboral!$A45)</f>
         <v/>
@@ -5303,7 +5313,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="str">
         <f>IF(Laboral!$A46="","",Laboral!$A46)</f>
         <v/>
@@ -5325,7 +5335,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="str">
         <f>IF(Laboral!$A47="","",Laboral!$A47)</f>
         <v/>
@@ -5347,7 +5357,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="str">
         <f>IF(Laboral!$A48="","",Laboral!$A48)</f>
         <v/>
@@ -5369,7 +5379,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="str">
         <f>IF(Laboral!$A49="","",Laboral!$A49)</f>
         <v/>
@@ -5391,7 +5401,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="str">
         <f>IF(Laboral!$A50="","",Laboral!$A50)</f>
         <v/>
@@ -5422,20 +5432,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="1" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
@@ -5449,7 +5460,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>IFERROR(VLOOKUP(Academica!$A5,cargos,2,FALSE),"")</f>
         <v>1</v>
@@ -5467,7 +5478,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A6,cargos,2,FALSE),"")</f>
         <v/>
@@ -5485,7 +5496,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A7,cargos,2,FALSE),"")</f>
         <v/>
@@ -5503,7 +5514,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A8,cargos,2,FALSE),"")</f>
         <v/>
@@ -5521,7 +5532,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A9,cargos,2,FALSE),"")</f>
         <v/>
@@ -5539,7 +5550,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A10,cargos,2,FALSE),"")</f>
         <v/>
@@ -5557,7 +5568,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A11,cargos,2,FALSE),"")</f>
         <v/>
@@ -5575,7 +5586,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A12,cargos,2,FALSE),"")</f>
         <v/>
@@ -5593,7 +5604,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A13,cargos,2,FALSE),"")</f>
         <v/>
@@ -5611,7 +5622,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A14,cargos,2,FALSE),"")</f>
         <v/>
@@ -5629,7 +5640,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A15,cargos,2,FALSE),"")</f>
         <v/>
@@ -5647,7 +5658,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A16,cargos,2,FALSE),"")</f>
         <v/>
@@ -5665,7 +5676,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A17,cargos,2,FALSE),"")</f>
         <v/>
@@ -5683,7 +5694,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A18,cargos,2,FALSE),"")</f>
         <v/>
@@ -5701,7 +5712,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A19,cargos,2,FALSE),"")</f>
         <v/>
@@ -5719,7 +5730,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A20,cargos,2,FALSE),"")</f>
         <v/>
@@ -5737,7 +5748,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A21,cargos,2,FALSE),"")</f>
         <v/>
@@ -5755,7 +5766,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A22,cargos,2,FALSE),"")</f>
         <v/>
@@ -5773,7 +5784,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A23,cargos,2,FALSE),"")</f>
         <v/>
@@ -5791,7 +5802,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A24,cargos,2,FALSE),"")</f>
         <v/>
@@ -5809,7 +5820,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A25,cargos,2,FALSE),"")</f>
         <v/>
@@ -5827,7 +5838,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A26,cargos,2,FALSE),"")</f>
         <v/>
@@ -5845,7 +5856,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A27,cargos,2,FALSE),"")</f>
         <v/>
@@ -5863,7 +5874,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A28,cargos,2,FALSE),"")</f>
         <v/>
@@ -5881,7 +5892,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A29,cargos,2,FALSE),"")</f>
         <v/>
@@ -5899,7 +5910,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A30,cargos,2,FALSE),"")</f>
         <v/>
@@ -5917,7 +5928,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A31,cargos,2,FALSE),"")</f>
         <v/>
@@ -5935,7 +5946,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A32,cargos,2,FALSE),"")</f>
         <v/>
@@ -5953,7 +5964,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A33,cargos,2,FALSE),"")</f>
         <v/>
@@ -5971,7 +5982,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A34,cargos,2,FALSE),"")</f>
         <v/>
@@ -5989,7 +6000,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A35,cargos,2,FALSE),"")</f>
         <v/>
@@ -6007,7 +6018,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A36,cargos,2,FALSE),"")</f>
         <v/>
@@ -6025,7 +6036,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A37,cargos,2,FALSE),"")</f>
         <v/>
@@ -6043,7 +6054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A38,cargos,2,FALSE),"")</f>
         <v/>
@@ -6061,7 +6072,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A39,cargos,2,FALSE),"")</f>
         <v/>
@@ -6079,7 +6090,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A40,cargos,2,FALSE),"")</f>
         <v/>
@@ -6097,7 +6108,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A41,cargos,2,FALSE),"")</f>
         <v/>
@@ -6115,7 +6126,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A42,cargos,2,FALSE),"")</f>
         <v/>
@@ -6133,7 +6144,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A43,cargos,2,FALSE),"")</f>
         <v/>
@@ -6151,7 +6162,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A44,cargos,2,FALSE),"")</f>
         <v/>
@@ -6169,7 +6180,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A45,cargos,2,FALSE),"")</f>
         <v/>
@@ -6187,7 +6198,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A46,cargos,2,FALSE),"")</f>
         <v/>
@@ -6205,7 +6216,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A47,cargos,2,FALSE),"")</f>
         <v/>
@@ -6223,7 +6234,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A48,cargos,2,FALSE),"")</f>
         <v/>
@@ -6241,7 +6252,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A49,cargos,2,FALSE),"")</f>
         <v/>
@@ -6259,7 +6270,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A50,cargos,2,FALSE),"")</f>
         <v/>
@@ -6277,7 +6288,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A51,cargos,2,FALSE),"")</f>
         <v/>
@@ -6295,7 +6306,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A52,cargos,2,FALSE),"")</f>
         <v/>
@@ -6313,7 +6324,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>IFERROR(VLOOKUP(Academica!$A53,cargos,2,FALSE),"")</f>
         <v/>
@@ -6339,21 +6350,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>161</v>
       </c>
@@ -6367,7 +6379,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(Certificaciones!$A5="","",Certificaciones!$A5)</f>
         <v/>
@@ -6385,7 +6397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(Certificaciones!$A6="","",Certificaciones!$A6)</f>
         <v/>
@@ -6403,7 +6415,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(Certificaciones!$A7="","",Certificaciones!$A7)</f>
         <v/>
@@ -6421,7 +6433,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(Certificaciones!$A8="","",Certificaciones!$A8)</f>
         <v/>
@@ -6439,7 +6451,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(Certificaciones!$A9="","",Certificaciones!$A9)</f>
         <v/>
@@ -6457,7 +6469,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(Certificaciones!$A10="","",Certificaciones!$A10)</f>
         <v/>
@@ -6475,7 +6487,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(Certificaciones!$A11="","",Certificaciones!$A11)</f>
         <v/>
@@ -6493,7 +6505,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(Certificaciones!$A12="","",Certificaciones!$A12)</f>
         <v/>
@@ -6511,7 +6523,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(Certificaciones!$A13="","",Certificaciones!$A13)</f>
         <v/>
@@ -6529,7 +6541,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(Certificaciones!$A14="","",Certificaciones!$A14)</f>
         <v/>
@@ -6547,7 +6559,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(Certificaciones!$A15="","",Certificaciones!$A15)</f>
         <v/>
@@ -6565,7 +6577,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(Certificaciones!$A16="","",Certificaciones!$A16)</f>
         <v/>
@@ -6583,7 +6595,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(Certificaciones!$A17="","",Certificaciones!$A17)</f>
         <v/>
@@ -6601,7 +6613,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(Certificaciones!$A18="","",Certificaciones!$A18)</f>
         <v/>
@@ -6619,7 +6631,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(Certificaciones!$A19="","",Certificaciones!$A19)</f>
         <v/>
@@ -6637,7 +6649,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(Certificaciones!$A20="","",Certificaciones!$A20)</f>
         <v/>
@@ -6655,7 +6667,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(Certificaciones!$A21="","",Certificaciones!$A21)</f>
         <v/>
@@ -6673,7 +6685,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(Certificaciones!$A22="","",Certificaciones!$A22)</f>
         <v/>
@@ -6691,7 +6703,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(Certificaciones!$A23="","",Certificaciones!$A23)</f>
         <v/>
@@ -6709,7 +6721,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF(Certificaciones!$A24="","",Certificaciones!$A24)</f>
         <v/>
@@ -6727,7 +6739,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF(Certificaciones!$A25="","",Certificaciones!$A25)</f>
         <v/>
@@ -6745,7 +6757,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF(Certificaciones!$A26="","",Certificaciones!$A26)</f>
         <v/>
@@ -6763,7 +6775,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF(Certificaciones!$A27="","",Certificaciones!$A27)</f>
         <v/>
@@ -6781,7 +6793,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF(Certificaciones!$A28="","",Certificaciones!$A28)</f>
         <v/>
@@ -6799,7 +6811,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF(Certificaciones!$A29="","",Certificaciones!$A29)</f>
         <v/>
@@ -6817,7 +6829,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF(Certificaciones!$A30="","",Certificaciones!$A30)</f>
         <v/>
@@ -6835,7 +6847,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF(Certificaciones!$A31="","",Certificaciones!$A31)</f>
         <v/>
@@ -6853,7 +6865,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF(Certificaciones!$A32="","",Certificaciones!$A32)</f>
         <v/>
@@ -6871,7 +6883,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF(Certificaciones!$A33="","",Certificaciones!$A33)</f>
         <v/>
@@ -6889,7 +6901,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF(Certificaciones!$A34="","",Certificaciones!$A34)</f>
         <v/>
@@ -6907,7 +6919,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF(Certificaciones!$A35="","",Certificaciones!$A35)</f>
         <v/>
@@ -6925,7 +6937,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF(Certificaciones!$A36="","",Certificaciones!$A36)</f>
         <v/>
@@ -6943,7 +6955,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF(Certificaciones!$A37="","",Certificaciones!$A37)</f>
         <v/>
@@ -6961,7 +6973,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IF(Certificaciones!$A38="","",Certificaciones!$A38)</f>
         <v/>
@@ -6979,7 +6991,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IF(Certificaciones!$A39="","",Certificaciones!$A39)</f>
         <v/>
@@ -6997,7 +7009,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IF(Certificaciones!$A40="","",Certificaciones!$A40)</f>
         <v/>
@@ -7015,7 +7027,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IF(Certificaciones!$A41="","",Certificaciones!$A41)</f>
         <v/>
@@ -7033,7 +7045,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF(Certificaciones!$A42="","",Certificaciones!$A42)</f>
         <v/>
@@ -7051,7 +7063,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF(Certificaciones!$A43="","",Certificaciones!$A43)</f>
         <v/>
@@ -7069,7 +7081,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IF(Certificaciones!$A44="","",Certificaciones!$A44)</f>
         <v/>
@@ -7087,7 +7099,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IF(Certificaciones!$A45="","",Certificaciones!$A45)</f>
         <v/>
@@ -7105,7 +7117,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>IF(Certificaciones!$A46="","",Certificaciones!$A46)</f>
         <v/>
@@ -7123,7 +7135,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IF(Certificaciones!$A47="","",Certificaciones!$A47)</f>
         <v/>
@@ -7141,7 +7153,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>IF(Certificaciones!$A48="","",Certificaciones!$A48)</f>
         <v/>
@@ -7159,7 +7171,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF(Certificaciones!$A49="","",Certificaciones!$A49)</f>
         <v/>
@@ -7177,7 +7189,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF(Certificaciones!$A50="","",Certificaciones!$A50)</f>
         <v/>
@@ -7195,7 +7207,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>IF(Certificaciones!$A51="","",Certificaciones!$A51)</f>
         <v/>
@@ -7213,7 +7225,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>IF(Certificaciones!$A52="","",Certificaciones!$A52)</f>
         <v/>
@@ -7231,7 +7243,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>IF(Certificaciones!$A53="","",Certificaciones!$A53)</f>
         <v/>

</xml_diff>